<commit_message>
updated app.py for hosting ready code
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -170,7 +170,7 @@
     <t>Stage4</t>
   </si>
   <si>
-    <t>Test Jhon6</t>
+    <t>Test Jhon8</t>
   </si>
   <si>
     <t>Restaurant</t>
@@ -218,7 +218,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Test Jhon7</t>
+    <t>Test Jhon9</t>
   </si>
   <si>
     <t>Accommodation</t>
@@ -1401,7 +1401,7 @@
   <dimension ref="A1:AT3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>

</xml_diff>